<commit_message>
version for hazard workshop
</commit_message>
<xml_diff>
--- a/rmtk/vulnerability/tests/NSP/checked_functions.xlsx
+++ b/rmtk/vulnerability/tests/NSP/checked_functions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>assign_damage</t>
   </si>
@@ -42,9 +42,6 @@
     <t>DF_method</t>
   </si>
   <si>
-    <t>getspo</t>
-  </si>
-  <si>
     <t>spo2ida</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>process_an1</t>
+  </si>
+  <si>
+    <t>getspo2ida_parameters</t>
   </si>
 </sst>
 </file>
@@ -461,20 +461,25 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -482,7 +487,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -499,7 +504,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -516,7 +521,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -527,18 +532,24 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vulnerability test on going
</commit_message>
<xml_diff>
--- a/rmtk/vulnerability/tests/NSP/checked_functions.xlsx
+++ b/rmtk/vulnerability/tests/NSP/checked_functions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>assign_damage</t>
   </si>
@@ -461,7 +461,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -495,6 +495,9 @@
       <c r="E2" t="s">
         <v>0</v>
       </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">

</xml_diff>